<commit_message>
ajustes nas fórmulas de logistica
</commit_message>
<xml_diff>
--- a/app/Dash_Logistica/kpis_luiz/planilha/WQ4 - Estoque Mercadorias Cliente WMS - cliente 2.xlsx
+++ b/app/Dash_Logistica/kpis_luiz/planilha/WQ4 - Estoque Mercadorias Cliente WMS - cliente 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hausz\Desktop\Projetos\2022\06_Junho\Backend_Flask\app\Dash_Logistica\kpis_luiz\planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCBFB7B-403E-4C61-8556-096E1DC5A271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FA4DBF-3943-46FE-AA22-A289D6E3553F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7538,30 +7538,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1085" workbookViewId="0">
-      <selection activeCell="G1096" sqref="G1096"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1078" workbookViewId="0">
+      <selection activeCell="A1106" sqref="A1106:XFD1106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7657,19 +7657,19 @@
         <v>0</v>
       </c>
       <c r="N2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="5">
         <v>0</v>
       </c>
       <c r="Q2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7709,19 +7709,19 @@
         <v>0</v>
       </c>
       <c r="N3" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O3" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3" s="5">
         <v>0</v>
       </c>
       <c r="Q3" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R3" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -10887,10 +10887,10 @@
         <v>8</v>
       </c>
       <c r="P64" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q64" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R64" s="6">
         <v>91</v>
@@ -11043,10 +11043,10 @@
         <v>2</v>
       </c>
       <c r="P67" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q67" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R67" s="6">
         <v>1</v>
@@ -11407,10 +11407,10 @@
         <v>22</v>
       </c>
       <c r="P74" s="5">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Q74" s="5">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="R74" s="6">
         <v>12</v>
@@ -14163,10 +14163,10 @@
         <v>1</v>
       </c>
       <c r="P127" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q127" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R127" s="6">
         <v>2</v>
@@ -15099,10 +15099,10 @@
         <v>92</v>
       </c>
       <c r="P145" s="5">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="Q145" s="5">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="R145" s="6">
         <v>115</v>
@@ -17023,10 +17023,10 @@
         <v>2</v>
       </c>
       <c r="P182" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q182" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R182" s="6">
         <v>5</v>
@@ -17855,10 +17855,10 @@
         <v>3</v>
       </c>
       <c r="P198" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q198" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R198" s="6">
         <v>1</v>
@@ -19363,10 +19363,10 @@
         <v>1</v>
       </c>
       <c r="P227" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q227" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R227" s="6">
         <v>7</v>
@@ -21400,7 +21400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="267" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
         <v>547</v>
       </c>
@@ -22483,10 +22483,10 @@
         <v>2</v>
       </c>
       <c r="P287" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q287" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R287" s="6">
         <v>0</v>
@@ -23939,10 +23939,10 @@
         <v>2</v>
       </c>
       <c r="P315" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q315" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R315" s="6">
         <v>0</v>
@@ -24251,10 +24251,10 @@
         <v>10</v>
       </c>
       <c r="P321" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q321" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R321" s="6">
         <v>0</v>
@@ -24615,10 +24615,10 @@
         <v>32</v>
       </c>
       <c r="P328" s="5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="Q328" s="5">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="R328" s="6">
         <v>198</v>
@@ -26169,19 +26169,19 @@
         <v>0</v>
       </c>
       <c r="N358" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O358" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P358" s="5">
         <v>3</v>
       </c>
       <c r="Q358" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R358" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="359" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -26903,10 +26903,10 @@
         <v>1</v>
       </c>
       <c r="P372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q372" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R372" s="6">
         <v>0</v>
@@ -28567,10 +28567,10 @@
         <v>8</v>
       </c>
       <c r="P404" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q404" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R404" s="6">
         <v>68</v>
@@ -29243,10 +29243,10 @@
         <v>2</v>
       </c>
       <c r="P417" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q417" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R417" s="6">
         <v>10</v>
@@ -30595,10 +30595,10 @@
         <v>16</v>
       </c>
       <c r="P443" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q443" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R443" s="6">
         <v>16</v>
@@ -30745,19 +30745,19 @@
         <v>0</v>
       </c>
       <c r="N446" s="5">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="O446" s="5">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="P446" s="5">
         <v>13</v>
       </c>
       <c r="Q446" s="5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="R446" s="6">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="447" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31115,10 +31115,10 @@
         <v>2</v>
       </c>
       <c r="P453" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q453" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R453" s="6">
         <v>2</v>
@@ -32311,10 +32311,10 @@
         <v>46</v>
       </c>
       <c r="P476" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q476" s="5">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="R476" s="6">
         <v>121</v>
@@ -32363,10 +32363,10 @@
         <v>70</v>
       </c>
       <c r="P477" s="5">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="Q477" s="5">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="R477" s="6">
         <v>161</v>
@@ -32467,10 +32467,10 @@
         <v>16</v>
       </c>
       <c r="P479" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="Q479" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="R479" s="6">
         <v>64</v>
@@ -33091,10 +33091,10 @@
         <v>2</v>
       </c>
       <c r="P491" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q491" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R491" s="6">
         <v>0</v>
@@ -33351,10 +33351,10 @@
         <v>12</v>
       </c>
       <c r="P496" s="5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Q496" s="5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="R496" s="6">
         <v>5</v>
@@ -34073,19 +34073,19 @@
         <v>0</v>
       </c>
       <c r="N510" s="5">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="O510" s="5">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="P510" s="5">
         <v>0</v>
       </c>
       <c r="Q510" s="5">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="R510" s="6">
-        <v>150</v>
+        <v>57</v>
       </c>
     </row>
     <row r="511" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -34905,19 +34905,19 @@
         <v>0</v>
       </c>
       <c r="N526" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O526" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P526" s="5">
         <v>0</v>
       </c>
       <c r="Q526" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R526" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="527" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -36055,10 +36055,10 @@
         <v>1</v>
       </c>
       <c r="P548" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q548" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R548" s="6">
         <v>5</v>
@@ -36679,10 +36679,10 @@
         <v>64</v>
       </c>
       <c r="P560" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q560" s="5">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="R560" s="6">
         <v>358</v>
@@ -36991,10 +36991,10 @@
         <v>24</v>
       </c>
       <c r="P566" s="5">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q566" s="5">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="R566" s="6">
         <v>0</v>
@@ -41515,10 +41515,10 @@
         <v>15</v>
       </c>
       <c r="P653" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Q653" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R653" s="6">
         <v>36</v>
@@ -42295,10 +42295,10 @@
         <v>1</v>
       </c>
       <c r="P668" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q668" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R668" s="6">
         <v>0</v>
@@ -42399,10 +42399,10 @@
         <v>1</v>
       </c>
       <c r="P670" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q670" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R670" s="6">
         <v>0</v>
@@ -42607,10 +42607,10 @@
         <v>1</v>
       </c>
       <c r="P674" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q674" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R674" s="6">
         <v>0</v>
@@ -43075,10 +43075,10 @@
         <v>2</v>
       </c>
       <c r="P683" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q683" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R683" s="6">
         <v>0</v>
@@ -43439,10 +43439,10 @@
         <v>1</v>
       </c>
       <c r="P690" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q690" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R690" s="6">
         <v>0</v>
@@ -44167,10 +44167,10 @@
         <v>3</v>
       </c>
       <c r="P704" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q704" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R704" s="6">
         <v>13</v>
@@ -44791,10 +44791,10 @@
         <v>1</v>
       </c>
       <c r="P716" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q716" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R716" s="6">
         <v>0</v>
@@ -45883,10 +45883,10 @@
         <v>1</v>
       </c>
       <c r="P737" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q737" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R737" s="6">
         <v>1</v>
@@ -46672,7 +46672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="753" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="753" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A753" s="4" t="s">
         <v>1507</v>
       </c>
@@ -46724,7 +46724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="754" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="754" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A754" s="4" t="s">
         <v>1509</v>
       </c>
@@ -46776,7 +46776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="755" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="755" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A755" s="4" t="s">
         <v>1511</v>
       </c>
@@ -46828,7 +46828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="756" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="756" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A756" s="4" t="s">
         <v>1513</v>
       </c>
@@ -47348,7 +47348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="766" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="766" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A766" s="4" t="s">
         <v>1533</v>
       </c>
@@ -47495,16 +47495,16 @@
         <v>2</v>
       </c>
       <c r="P768" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q768" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R768" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="769" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="769" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A769" s="4" t="s">
         <v>1539</v>
       </c>
@@ -47556,7 +47556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="770" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="770" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A770" s="4" t="s">
         <v>1541</v>
       </c>
@@ -47703,10 +47703,10 @@
         <v>2</v>
       </c>
       <c r="P772" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q772" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R772" s="6">
         <v>1</v>
@@ -48492,7 +48492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="788" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="788" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A788" s="4" t="s">
         <v>1577</v>
       </c>
@@ -48587,10 +48587,10 @@
         <v>3</v>
       </c>
       <c r="P789" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q789" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R789" s="6">
         <v>17</v>
@@ -48648,7 +48648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="791" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="791" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A791" s="4" t="s">
         <v>1583</v>
       </c>
@@ -50043,10 +50043,10 @@
         <v>2</v>
       </c>
       <c r="P817" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q817" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R817" s="6">
         <v>20</v>
@@ -50563,10 +50563,10 @@
         <v>3</v>
       </c>
       <c r="P827" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q827" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R827" s="6">
         <v>12</v>
@@ -51187,10 +51187,10 @@
         <v>9</v>
       </c>
       <c r="P839" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q839" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R839" s="6">
         <v>4</v>
@@ -51863,10 +51863,10 @@
         <v>1</v>
       </c>
       <c r="P852" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q852" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R852" s="6">
         <v>0</v>
@@ -52019,10 +52019,10 @@
         <v>4</v>
       </c>
       <c r="P855" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q855" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R855" s="6">
         <v>1</v>
@@ -53059,10 +53059,10 @@
         <v>1</v>
       </c>
       <c r="P875" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q875" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R875" s="6">
         <v>1</v>
@@ -53371,10 +53371,10 @@
         <v>1</v>
       </c>
       <c r="P881" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q881" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R881" s="6">
         <v>0</v>
@@ -53683,10 +53683,10 @@
         <v>2</v>
       </c>
       <c r="P887" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q887" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R887" s="6">
         <v>2</v>
@@ -53891,10 +53891,10 @@
         <v>1</v>
       </c>
       <c r="P891" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q891" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R891" s="6">
         <v>0</v>
@@ -54879,10 +54879,10 @@
         <v>1</v>
       </c>
       <c r="P910" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q910" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R910" s="6">
         <v>0</v>
@@ -54931,10 +54931,10 @@
         <v>5</v>
       </c>
       <c r="P911" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q911" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R911" s="6">
         <v>7</v>
@@ -55295,10 +55295,10 @@
         <v>3</v>
       </c>
       <c r="P918" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q918" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R918" s="6">
         <v>5</v>
@@ -55711,10 +55711,10 @@
         <v>1</v>
       </c>
       <c r="P926" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q926" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R926" s="6">
         <v>0</v>
@@ -56439,10 +56439,10 @@
         <v>2</v>
       </c>
       <c r="P940" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q940" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R940" s="6">
         <v>3</v>
@@ -56959,10 +56959,10 @@
         <v>3</v>
       </c>
       <c r="P950" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q950" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R950" s="6">
         <v>3</v>
@@ -57479,10 +57479,10 @@
         <v>2</v>
       </c>
       <c r="P960" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q960" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R960" s="6">
         <v>4</v>
@@ -57687,10 +57687,10 @@
         <v>2</v>
       </c>
       <c r="P964" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q964" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R964" s="6">
         <v>0</v>
@@ -57739,10 +57739,10 @@
         <v>2</v>
       </c>
       <c r="P965" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q965" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R965" s="6">
         <v>3</v>
@@ -58103,10 +58103,10 @@
         <v>3</v>
       </c>
       <c r="P972" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q972" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R972" s="6">
         <v>3</v>
@@ -58155,10 +58155,10 @@
         <v>4</v>
       </c>
       <c r="P973" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q973" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R973" s="6">
         <v>1</v>
@@ -58623,10 +58623,10 @@
         <v>1</v>
       </c>
       <c r="P982" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q982" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R982" s="6">
         <v>0</v>
@@ -58779,10 +58779,10 @@
         <v>3</v>
       </c>
       <c r="P985" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q985" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R985" s="6">
         <v>0</v>
@@ -58935,10 +58935,10 @@
         <v>6</v>
       </c>
       <c r="P988" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q988" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R988" s="6">
         <v>0</v>
@@ -59091,10 +59091,10 @@
         <v>3</v>
       </c>
       <c r="P991" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q991" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R991" s="6">
         <v>1</v>
@@ -60859,10 +60859,10 @@
         <v>10</v>
       </c>
       <c r="P1025" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q1025" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R1025" s="6">
         <v>0</v>
@@ -64343,10 +64343,10 @@
         <v>2</v>
       </c>
       <c r="P1092" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q1092" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R1092" s="6">
         <v>2</v>
@@ -64603,10 +64603,10 @@
         <v>2</v>
       </c>
       <c r="P1097" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q1097" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R1097" s="6">
         <v>1</v>
@@ -64820,7 +64820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1102" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1102" spans="1:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1102" s="4" t="s">
         <v>2185</v>
       </c>

</xml_diff>